<commit_message>
Add column test data from October 2023
</commit_message>
<xml_diff>
--- a/data/lime_products.xlsx
+++ b/data/lime_products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\liming_data\tidy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E54884BC-604F-4F04-A11C-3C0421ADF6F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E32B95-5B10-4F94-8EFD-0A5E61CBF498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6981859C-58BB-46A6-A870-23E91445E341}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6981859C-58BB-46A6-A870-23E91445E341}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Property</t>
   </si>
@@ -129,7 +134,13 @@
     <t>Miljøkalk VK3</t>
   </si>
   <si>
-    <t>SK2</t>
+    <t>Microdol1</t>
+  </si>
+  <si>
+    <t>Microdol5</t>
+  </si>
+  <si>
+    <t>SK2 (old data)</t>
   </si>
 </sst>
 </file>
@@ -498,21 +509,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDEC087-0582-4E3C-ADF0-FAA6607A2EDC}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="50" width="15.7109375" customWidth="1"/>
+    <col min="3" max="42" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,8 +539,14 @@
       <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -537,16 +554,22 @@
         <v>16</v>
       </c>
       <c r="C2">
-        <v>38.5</v>
+        <v>39.6</v>
       </c>
       <c r="D2">
-        <v>39</v>
+        <v>39.6</v>
       </c>
       <c r="E2">
+        <v>21.5</v>
+      </c>
+      <c r="F2">
+        <v>21.5</v>
+      </c>
+      <c r="G2">
         <v>33.200000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -554,16 +577,22 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E3">
+        <v>12.8</v>
+      </c>
+      <c r="F3">
+        <v>12.8</v>
+      </c>
+      <c r="G3">
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -577,10 +606,16 @@
         <v>0.7</v>
       </c>
       <c r="E4">
+        <v>0.7</v>
+      </c>
+      <c r="F4">
+        <v>0.7</v>
+      </c>
+      <c r="G4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -594,10 +629,16 @@
         <v>2</v>
       </c>
       <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -605,16 +646,22 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>70.400000000000006</v>
+        <v>64</v>
       </c>
       <c r="D6">
-        <v>81.900000000000006</v>
+        <v>61.2</v>
       </c>
       <c r="E6">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="F6">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="G6">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -622,16 +669,22 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>51.2</v>
+        <v>48.6</v>
       </c>
       <c r="D7">
-        <v>63.4</v>
+        <v>60.5</v>
       </c>
       <c r="E7">
+        <v>76.2</v>
+      </c>
+      <c r="F7">
+        <v>46.1</v>
+      </c>
+      <c r="G7">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -639,16 +692,22 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>44</v>
+        <v>50.3</v>
       </c>
       <c r="D8">
-        <v>58.4</v>
+        <v>60.2</v>
       </c>
       <c r="E8">
+        <v>25.1</v>
+      </c>
+      <c r="F8">
+        <v>33.4</v>
+      </c>
+      <c r="G8">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -656,16 +715,22 @@
         <v>23</v>
       </c>
       <c r="C9">
-        <v>42.3</v>
+        <v>43</v>
       </c>
       <c r="D9">
-        <v>51.6</v>
+        <v>51.7</v>
       </c>
       <c r="E9">
+        <v>25.6</v>
+      </c>
+      <c r="F9">
+        <v>25.3</v>
+      </c>
+      <c r="G9">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -673,16 +738,22 @@
         <v>24</v>
       </c>
       <c r="C10">
-        <v>37.799999999999997</v>
+        <v>34.9</v>
       </c>
       <c r="D10">
-        <v>52.1</v>
+        <v>48.5</v>
       </c>
       <c r="E10">
+        <v>24.8</v>
+      </c>
+      <c r="F10">
+        <v>29.9</v>
+      </c>
+      <c r="G10">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -698,8 +769,14 @@
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -707,16 +784,22 @@
         <v>26</v>
       </c>
       <c r="C12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D12">
         <v>1.2</v>
       </c>
-      <c r="D12">
-        <v>1.3</v>
-      </c>
       <c r="E12">
+        <v>1.4</v>
+      </c>
+      <c r="F12">
+        <v>1.5</v>
+      </c>
+      <c r="G12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -724,16 +807,22 @@
         <v>27</v>
       </c>
       <c r="C13">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="D13">
+        <v>1.6</v>
+      </c>
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="E13">
+      <c r="F13">
+        <v>1.9</v>
+      </c>
+      <c r="G13">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -741,16 +830,22 @@
         <v>28</v>
       </c>
       <c r="C14">
+        <v>2.1</v>
+      </c>
+      <c r="D14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D14">
-        <v>2.2999999999999998</v>
-      </c>
       <c r="E14">
+        <v>2.1</v>
+      </c>
+      <c r="F14">
+        <v>2.8</v>
+      </c>
+      <c r="G14">
         <v>1.4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -758,12 +853,18 @@
         <v>29</v>
       </c>
       <c r="C15">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="D15">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="E15">
+        <v>3.1</v>
+      </c>
+      <c r="F15">
+        <v>3.8</v>
+      </c>
+      <c r="G15">
         <v>2.2999999999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update column test results for Microdol 1 and 5
</commit_message>
<xml_diff>
--- a/data/lime_products.xlsx
+++ b/data/lime_products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\liming_data\tidy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E32B95-5B10-4F94-8EFD-0A5E61CBF498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB589EF7-91F3-47BA-9E8C-F1C7109070C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6981859C-58BB-46A6-A870-23E91445E341}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6981859C-58BB-46A6-A870-23E91445E341}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,10 +652,10 @@
         <v>61.2</v>
       </c>
       <c r="E6">
-        <v>73.099999999999994</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="F6">
-        <v>70.599999999999994</v>
+        <v>81.3</v>
       </c>
       <c r="G6">
         <v>66</v>
@@ -675,10 +675,10 @@
         <v>60.5</v>
       </c>
       <c r="E7">
-        <v>76.2</v>
+        <v>45.2</v>
       </c>
       <c r="F7">
-        <v>46.1</v>
+        <v>50.1</v>
       </c>
       <c r="G7">
         <v>63</v>
@@ -698,10 +698,10 @@
         <v>60.2</v>
       </c>
       <c r="E8">
-        <v>25.1</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="F8">
-        <v>33.4</v>
+        <v>40.1</v>
       </c>
       <c r="G8">
         <v>60</v>
@@ -721,10 +721,10 @@
         <v>51.7</v>
       </c>
       <c r="E9">
-        <v>25.6</v>
+        <v>29.3</v>
       </c>
       <c r="F9">
-        <v>25.3</v>
+        <v>33.6</v>
       </c>
       <c r="G9">
         <v>58</v>
@@ -744,10 +744,10 @@
         <v>48.5</v>
       </c>
       <c r="E10">
-        <v>24.8</v>
+        <v>29.6</v>
       </c>
       <c r="F10">
-        <v>29.9</v>
+        <v>35.6</v>
       </c>
       <c r="G10">
         <v>56</v>

</xml_diff>

<commit_message>
Add "Standard Kalk Kat3" to products.xlsx
</commit_message>
<xml_diff>
--- a/data/lime_products.xlsx
+++ b/data/lime_products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7629AABE-C6D7-4AFF-BE5D-9614A3EAD8FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE8EC99-A422-4893-A4DB-A9D21CDB2E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6981859C-58BB-46A6-A870-23E91445E341}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6981859C-58BB-46A6-A870-23E91445E341}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Property</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Omya Hustadmarmor Biokalk</t>
+  </si>
+  <si>
+    <t>Standard Kalk Kat3</t>
   </si>
 </sst>
 </file>
@@ -222,9 +225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -262,7 +265,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -368,7 +371,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -510,7 +513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -518,11 +521,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDEC087-0582-4E3C-ADF0-FAA6607A2EDC}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,10 +535,11 @@
     <col min="3" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="9" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="42" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="42" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,8 +570,11 @@
       <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -598,8 +605,11 @@
       <c r="J2">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -630,8 +640,11 @@
       <c r="J3">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -662,8 +675,11 @@
       <c r="J4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -694,8 +710,11 @@
       <c r="J5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -726,8 +745,11 @@
       <c r="J6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>61.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -758,8 +780,11 @@
       <c r="J7">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -790,8 +815,11 @@
       <c r="J8">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>60.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -822,8 +850,11 @@
       <c r="J9">
         <v>92</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>51.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -854,8 +885,11 @@
       <c r="J10">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -886,8 +920,11 @@
       <c r="J11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -918,8 +955,11 @@
       <c r="J12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -950,8 +990,11 @@
       <c r="J13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -982,8 +1025,11 @@
       <c r="J14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1013,6 +1059,9 @@
       </c>
       <c r="J15">
         <v>1.2</v>
+      </c>
+      <c r="K15">
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove SK2 from products
</commit_message>
<xml_diff>
--- a/data/lime_products.xlsx
+++ b/data/lime_products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE8EC99-A422-4893-A4DB-A9D21CDB2E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999478BB-4388-486A-B9C6-4DA8ABFF6F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{6981859C-58BB-46A6-A870-23E91445E341}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Property</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Microdol5</t>
-  </si>
-  <si>
-    <t>SK2 (old data)</t>
   </si>
   <si>
     <t>Visnes Filterkalk Kat3</t>
@@ -521,25 +518,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDEC087-0582-4E3C-ADF0-FAA6607A2EDC}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="9" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="42" width="15.7109375" customWidth="1"/>
+    <col min="11" max="41" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,34 +544,31 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -588,13 +582,13 @@
         <v>39.6</v>
       </c>
       <c r="E2">
-        <v>21.5</v>
+        <v>39.6</v>
       </c>
       <c r="F2">
         <v>21.5</v>
       </c>
       <c r="G2">
-        <v>33.200000000000003</v>
+        <v>21.5</v>
       </c>
       <c r="H2">
         <v>39.700000000000003</v>
@@ -605,11 +599,8 @@
       <c r="J2">
         <v>27</v>
       </c>
-      <c r="K2">
-        <v>39.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -623,13 +614,13 @@
         <v>0.4</v>
       </c>
       <c r="E3">
-        <v>12.8</v>
+        <v>0.4</v>
       </c>
       <c r="F3">
         <v>12.8</v>
       </c>
       <c r="G3">
-        <v>1.4</v>
+        <v>12.8</v>
       </c>
       <c r="H3">
         <v>0.38</v>
@@ -640,11 +631,8 @@
       <c r="J3">
         <v>0.38</v>
       </c>
-      <c r="K3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -664,7 +652,7 @@
         <v>0.7</v>
       </c>
       <c r="G4">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="H4">
         <v>0.7</v>
@@ -675,11 +663,8 @@
       <c r="J4">
         <v>0.7</v>
       </c>
-      <c r="K4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -710,11 +695,8 @@
       <c r="J5">
         <v>2</v>
       </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -722,19 +704,19 @@
         <v>20</v>
       </c>
       <c r="C6">
+        <v>61.2</v>
+      </c>
+      <c r="D6">
         <v>64</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>61.2</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>66.099999999999994</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>81.3</v>
-      </c>
-      <c r="G6">
-        <v>66</v>
       </c>
       <c r="H6">
         <v>88</v>
@@ -745,11 +727,8 @@
       <c r="J6">
         <v>100</v>
       </c>
-      <c r="K6">
-        <v>61.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -757,19 +736,19 @@
         <v>21</v>
       </c>
       <c r="C7">
+        <v>60.5</v>
+      </c>
+      <c r="D7">
         <v>48.6</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>60.5</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>45.2</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>50.1</v>
-      </c>
-      <c r="G7">
-        <v>63</v>
       </c>
       <c r="H7">
         <v>74</v>
@@ -780,11 +759,8 @@
       <c r="J7">
         <v>97</v>
       </c>
-      <c r="K7">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -792,19 +768,19 @@
         <v>22</v>
       </c>
       <c r="C8">
+        <v>60.2</v>
+      </c>
+      <c r="D8">
         <v>50.3</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>60.2</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>32.799999999999997</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>40.1</v>
-      </c>
-      <c r="G8">
-        <v>60</v>
       </c>
       <c r="H8">
         <v>67</v>
@@ -815,11 +791,8 @@
       <c r="J8">
         <v>94</v>
       </c>
-      <c r="K8">
-        <v>60.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -827,19 +800,19 @@
         <v>23</v>
       </c>
       <c r="C9">
+        <v>51.7</v>
+      </c>
+      <c r="D9">
         <v>43</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>51.7</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>29.3</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>33.6</v>
-      </c>
-      <c r="G9">
-        <v>58</v>
       </c>
       <c r="H9">
         <v>64</v>
@@ -850,11 +823,8 @@
       <c r="J9">
         <v>92</v>
       </c>
-      <c r="K9">
-        <v>51.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -862,19 +832,19 @@
         <v>24</v>
       </c>
       <c r="C10">
+        <v>48.5</v>
+      </c>
+      <c r="D10">
         <v>34.9</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>48.5</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>29.6</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>35.6</v>
-      </c>
-      <c r="G10">
-        <v>56</v>
       </c>
       <c r="H10">
         <v>62</v>
@@ -885,11 +855,8 @@
       <c r="J10">
         <v>91</v>
       </c>
-      <c r="K10">
-        <v>48.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -920,11 +887,8 @@
       <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -932,19 +896,19 @@
         <v>26</v>
       </c>
       <c r="C12">
+        <v>1.2</v>
+      </c>
+      <c r="D12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1.2</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>1.4</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1.5</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
       </c>
       <c r="H12">
         <v>1.1000000000000001</v>
@@ -955,11 +919,8 @@
       <c r="J12">
         <v>1</v>
       </c>
-      <c r="K12">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -973,13 +934,13 @@
         <v>1.6</v>
       </c>
       <c r="E13">
+        <v>1.6</v>
+      </c>
+      <c r="F13">
         <v>2</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1.9</v>
-      </c>
-      <c r="G13">
-        <v>1.1000000000000001</v>
       </c>
       <c r="H13">
         <v>1.2</v>
@@ -990,11 +951,8 @@
       <c r="J13">
         <v>1</v>
       </c>
-      <c r="K13">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1002,19 +960,19 @@
         <v>28</v>
       </c>
       <c r="C14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D14">
         <v>2.1</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>2.1</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>2.8</v>
-      </c>
-      <c r="G14">
-        <v>1.4</v>
       </c>
       <c r="H14">
         <v>1.3</v>
@@ -1025,11 +983,8 @@
       <c r="J14">
         <v>1</v>
       </c>
-      <c r="K14">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1043,13 +998,13 @@
         <v>3.2</v>
       </c>
       <c r="E15">
+        <v>3.2</v>
+      </c>
+      <c r="F15">
         <v>3.1</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>3.8</v>
-      </c>
-      <c r="G15">
-        <v>2.2999999999999998</v>
       </c>
       <c r="H15">
         <v>1.6</v>
@@ -1059,9 +1014,6 @@
       </c>
       <c r="J15">
         <v>1.2</v>
-      </c>
-      <c r="K15">
-        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>